<commit_message>
Refactor prueba API y se agregó la prueba WEB
</commit_message>
<xml_diff>
--- a/src/data/Datos-pruebas.xlsx
+++ b/src/data/Datos-pruebas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielaalba/Documents/PlaywrightMonnet/challenge-automation-ga/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{188826E5-D400-5D46-A425-DD1F94AC24FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23954CC0-3A03-1849-876E-D4E10C3353C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-4120" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{11C48A19-DFE8-C948-8EFC-975104A98A53}"/>
   </bookViews>
@@ -42,22 +42,22 @@
     <t>abilities</t>
   </si>
   <si>
-    <t>bulbasaur</t>
-  </si>
-  <si>
-    <t>overgrow, chlorophyll</t>
+    <t>run-away, adaptability, anticipation</t>
+  </si>
+  <si>
+    <t>Charizard</t>
   </si>
   <si>
     <t>blaze, solar-power</t>
   </si>
   <si>
-    <t>charmander</t>
-  </si>
-  <si>
-    <t>ponyta</t>
-  </si>
-  <si>
-    <t>run-away, flash-fire, flame-body</t>
+    <t>Eevee</t>
+  </si>
+  <si>
+    <t>Pikachu</t>
+  </si>
+  <si>
+    <t>static, lightning-rod</t>
   </si>
 </sst>
 </file>
@@ -419,7 +419,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -441,29 +441,29 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>4</v>
+        <v>133</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>77</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>

</xml_diff>